<commit_message>
update readme and sample form
</commit_message>
<xml_diff>
--- a/extras/sample-form/Sample form - Display graph.xlsx
+++ b/extras/sample-form/Sample form - Display graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\display-graph\extras\sample-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A768F5-5926-4487-90D7-05A12620FF2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF968E60-F429-49E0-9311-6762AD624588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="19440" windowHeight="14385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="help-choices" sheetId="5" r:id="rId5"/>
     <sheet name="help-settings" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="1000" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2979,18 +2979,18 @@
     <t>display_graph</t>
   </si>
   <si>
-    <t xml:space="preserve">Welcome to this sample form for the display-graph field plug-in. The plug-in allows you to display a web-published graph from Google sheets in your form.&lt;br&gt; 
+    <t>Hint Message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to this sample form for the display-iframe field plug-in. The plug-in allows you to display a web-published graph from Google sheets, or other web content in an iframe, in your form. This demo displays graphs from Google Sheets.&lt;br&gt; 
 You can learn about &lt;a href="https://support.google.com/docs/answer/1047436?co=GENIE.Platform%3DDesktop&amp;hl=en" target="_blank"&gt;how to publish a chart here. &lt;/a&gt; 
 </t>
   </si>
   <si>
-    <t>custom-display-graph(link="https://docs.google.com/spreadsheets/d/e/2PACX-1vQnMZpxa6JZjIuM8I9yowgtuyrkXBDcP_ULnJoNHjuD7zGacUX0g4zVSmYnfaAD6rSCTPwvsiDKOmxb/pubchart?oid=1569534844&amp;format=interactive")</t>
-  </si>
-  <si>
-    <t>Hint Message</t>
-  </si>
-  <si>
-    <t>custom-display-graph(link="https://docs.google.com/spreadsheets/d/e/2PACX-1vQnMZpxa6JZjIuM8I9yowgtuyrkXBDcP_ULnJoNHjuD7zGacUX0g4zVSmYnfaAD6rSCTPwvsiDKOmxb/pubchart?oid=1099055857&amp;format=interactive")</t>
+    <t>custom-display-graph(link="https://docs.google.com/spreadsheets/d/e/2PACX-1vTD80eAbc3rcSYPu4hMoCOZDkyKZ0kD5SZ2FowYN-EXWlN0jrP4T22osV_P_9DgrJJum4FwFtt11NkX/pubchart?oid=201647898&amp;format=interactive")</t>
+  </si>
+  <si>
+    <t>custom-display-graph(link="https://docs.google.com/spreadsheets/d/e/2PACX-1vTD80eAbc3rcSYPu4hMoCOZDkyKZ0kD5SZ2FowYN-EXWlN0jrP4T22osV_P_9DgrJJum4FwFtt11NkX/pubchart?oid=148310736&amp;format=interactive")</t>
   </si>
 </sst>
 </file>
@@ -5217,10 +5217,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -5463,12 +5463,12 @@
         <v>370</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:27" s="44" customFormat="1">
       <c r="A13" s="42" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="B13" s="42" t="s">
         <v>369</v>
@@ -5477,11 +5477,11 @@
         <v>366</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G13" s="42"/>
       <c r="H13" s="43"/>
@@ -5503,7 +5503,7 @@
     </row>
     <row r="14" spans="1:27" s="44" customFormat="1">
       <c r="A14" s="42" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="B14" s="42" t="s">
         <v>368</v>
@@ -5512,7 +5512,7 @@
         <v>367</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42" t="s">
@@ -6047,7 +6047,7 @@
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2008121739</v>
+        <v>2009251031</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
@@ -6184,7 +6184,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="19" customFormat="1" ht="202.8">
+    <row r="6" spans="1:30" s="19" customFormat="1" ht="187.2">
       <c r="A6" s="18" t="s">
         <v>71</v>
       </c>
@@ -6502,7 +6502,7 @@
       <c r="AC14" s="23"/>
       <c r="AD14" s="23"/>
     </row>
-    <row r="15" spans="1:30" s="25" customFormat="1" ht="46.8">
+    <row r="15" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A15" s="23" t="s">
         <v>110</v>
       </c>
@@ -6582,7 +6582,7 @@
       <c r="AC16" s="23"/>
       <c r="AD16" s="23"/>
     </row>
-    <row r="17" spans="1:30" s="25" customFormat="1" ht="62.4">
+    <row r="17" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A17" s="23" t="s">
         <v>110</v>
       </c>
@@ -6702,7 +6702,7 @@
       <c r="AC19" s="23"/>
       <c r="AD19" s="23"/>
     </row>
-    <row r="20" spans="1:30" s="25" customFormat="1" ht="46.8">
+    <row r="20" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A20" s="23" t="s">
         <v>110</v>
       </c>
@@ -10373,7 +10373,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" s="19" customFormat="1" ht="312">
+    <row r="6" spans="1:8" s="19" customFormat="1" ht="296.39999999999998">
       <c r="A6" s="18" t="s">
         <v>360</v>
       </c>

</xml_diff>